<commit_message>
Working on t test
</commit_message>
<xml_diff>
--- a/Tables - ordinal - Control at T1 v. T2 - weight_a.xlsx
+++ b/Tables - ordinal - Control at T1 v. T2 - weight_a.xlsx
@@ -587,52 +587,40 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>2</v>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1079,52 +1067,40 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>2</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1375,52 +1351,40 @@
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>2</v>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1867,52 +1831,40 @@
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N19" t="n">
-        <v>2</v>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2359,52 +2311,40 @@
         <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N25" t="n">
-        <v>2</v>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2851,52 +2791,40 @@
         <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N31" t="n">
-        <v>2</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T31" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -3343,52 +3271,40 @@
         <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N37" t="n">
-        <v>2</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3737,52 +3653,40 @@
         <v>1</v>
       </c>
       <c r="I42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N42" t="n">
-        <v>2</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T42" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -4229,52 +4133,40 @@
         <v>1</v>
       </c>
       <c r="I48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N48" t="n">
-        <v>2</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T48" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="n">
+        <v>0</v>
+      </c>
+      <c r="T48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -4525,52 +4417,40 @@
         <v>1</v>
       </c>
       <c r="I52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N52" t="n">
-        <v>2</v>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T52" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="n">
+        <v>0</v>
+      </c>
+      <c r="T52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -5017,52 +4897,40 @@
         <v>1</v>
       </c>
       <c r="I58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N58" t="n">
-        <v>2</v>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T58" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="n">
+        <v>0</v>
+      </c>
+      <c r="T58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -5509,52 +5377,40 @@
         <v>1</v>
       </c>
       <c r="I64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N64" t="n">
-        <v>2</v>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T64" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O64" t="n">
+        <v>0</v>
+      </c>
+      <c r="P64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0</v>
+      </c>
+      <c r="R64" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -6001,52 +5857,40 @@
         <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N70" t="n">
-        <v>2</v>
-      </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P70" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R70" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S70" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T70" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0</v>
+      </c>
+      <c r="R70" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="n">
+        <v>0</v>
+      </c>
+      <c r="T70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -6493,52 +6337,40 @@
         <v>1</v>
       </c>
       <c r="I76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N76" t="n">
-        <v>2</v>
-      </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
-      </c>
-      <c r="T76" t="inlineStr">
-        <is>
-          <t>0 (P=0.050)</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>0</v>
+      </c>
+      <c r="R76" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" t="n">
+        <v>0</v>
+      </c>
+      <c r="T76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">

</xml_diff>